<commit_message>
Trial simulations; SST config files; updated bash script for convergence analysis
</commit_message>
<xml_diff>
--- a/Simulations/SimulationsLog.xlsx
+++ b/Simulations/SimulationsLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\OneDrive - Politecnico di Milano\Documenti\Università\2022-2023 - Quinto Anno\Computational Fluid Dynamics\Project\progetto_CFD\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A96766-BD4C-4529-B07D-210F34FF2815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF34605A-9E91-4914-90A3-FC30ABBDA0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid Properties &amp; Calculations" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="84">
   <si>
     <t>Mesh</t>
   </si>
@@ -80,9 +80,6 @@
     <t>FDS - MUSCL OFF</t>
   </si>
   <si>
-    <t>Folder: Space Convergence</t>
-  </si>
-  <si>
     <t>Simulation ID</t>
   </si>
   <si>
@@ -246,6 +243,54 @@
   </si>
   <si>
     <t>postStall AOA</t>
+  </si>
+  <si>
+    <t>MESH PROPERTIES</t>
+  </si>
+  <si>
+    <t>meshG1</t>
+  </si>
+  <si>
+    <t>meshG2</t>
+  </si>
+  <si>
+    <t>meshG4</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>meshG3</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Folder: SC</t>
+  </si>
+  <si>
+    <t>Folder: P</t>
+  </si>
+  <si>
+    <t>SST-V2033m-VORTICITY-SUSTAINING with std boundary conditions</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>SST-V2033m with std boundary conditions</t>
   </si>
 </sst>
 </file>
@@ -297,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,8 +373,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -634,11 +685,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -723,6 +787,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1005,140 +1073,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB05BFA5-83D5-460F-8809-94ABF6EE4EEF}">
-  <dimension ref="B1:D41"/>
+  <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="10">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H2" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="10">
+        <v>40176</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="11">
         <v>1.5999999999999999E-5</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="12">
         <f>D3*D2</f>
         <v>1.9199999999999999E-5</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4">
         <v>1.008</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="12">
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>26</v>
-      </c>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="13">
         <f>D8*D3/D5</f>
         <v>9.5238095238095237</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>25</v>
+      </c>
       <c r="C11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="15">
         <f>D9*40/D3</f>
         <v>23809523.80952381</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12">
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D14" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="12">
         <v>0.1</v>
@@ -1146,7 +1239,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="17">
         <f>D12</f>
@@ -1155,7 +1248,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="17">
         <f>D13</f>
@@ -1164,57 +1257,56 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="17">
-        <f>D15/D14/D11</f>
-        <v>4.2000000000000003E-13</v>
+        <f>SQRT(D15/D14/D11)</f>
+        <v>5.2915026221291808E-7</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="19">
-        <f>D16/D14/D11</f>
-        <v>4.2000000000000004E-9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SQRT(D16/D14/D11)</f>
+        <v>5.2915026221291811E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D22" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="C24" s="9" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="D24" s="28">
         <v>0.21043799999999999</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="29">
         <v>1.2942340000000001</v>
@@ -1222,10 +1314,10 @@
     </row>
     <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1284,13 +1376,13 @@
   <dimension ref="B1:H56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -1302,10 +1394,10 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>2</v>
@@ -1317,10 +1409,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1337,7 +1429,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>7</v>
@@ -1357,7 +1449,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>7</v>
@@ -1377,7 +1469,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>7</v>
@@ -1397,7 +1489,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>7</v>
@@ -1405,7 +1497,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="36">
         <v>9</v>
@@ -1414,10 +1506,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>7</v>
@@ -1425,7 +1517,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3">
         <v>9</v>
@@ -1434,10 +1526,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>7</v>
@@ -1445,7 +1537,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3">
         <v>9</v>
@@ -1454,10 +1546,10 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>7</v>
@@ -1465,7 +1557,7 @@
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="5">
         <v>9</v>
@@ -1474,10 +1566,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>7</v>
@@ -1485,7 +1577,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="36">
         <v>9</v>
@@ -1494,10 +1586,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>7</v>
@@ -1505,7 +1597,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3">
         <v>9</v>
@@ -1514,10 +1606,10 @@
         <v>4</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>7</v>
@@ -1525,7 +1617,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3">
         <v>9</v>
@@ -1534,10 +1626,10 @@
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>7</v>
@@ -1545,7 +1637,7 @@
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="37">
         <v>9</v>
@@ -1554,10 +1646,10 @@
         <v>6</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>7</v>
@@ -1565,7 +1657,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="36">
         <v>18</v>
@@ -1577,7 +1669,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>7</v>
@@ -1585,7 +1677,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3">
         <v>18</v>
@@ -1597,7 +1689,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>7</v>
@@ -1605,7 +1697,7 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3">
         <v>18</v>
@@ -1617,7 +1709,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>7</v>
@@ -1625,7 +1717,7 @@
     </row>
     <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="37">
         <v>18</v>
@@ -1637,7 +1729,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>7</v>
@@ -1645,7 +1737,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="36">
         <v>18</v>
@@ -1654,10 +1746,10 @@
         <v>3</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>7</v>
@@ -1665,7 +1757,7 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3">
         <v>18</v>
@@ -1674,10 +1766,10 @@
         <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>7</v>
@@ -1685,7 +1777,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3">
         <v>18</v>
@@ -1694,10 +1786,10 @@
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>7</v>
@@ -1705,7 +1797,7 @@
     </row>
     <row r="22" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="37">
         <v>18</v>
@@ -1714,10 +1806,10 @@
         <v>6</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="24" t="s">
         <v>7</v>
@@ -1725,7 +1817,7 @@
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="36">
         <v>18</v>
@@ -1734,10 +1826,10 @@
         <v>3</v>
       </c>
       <c r="F23" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>7</v>
@@ -1745,7 +1837,7 @@
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="3">
         <v>18</v>
@@ -1754,10 +1846,10 @@
         <v>4</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>7</v>
@@ -1765,7 +1857,7 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="3">
         <v>18</v>
@@ -1774,10 +1866,10 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>7</v>
@@ -1785,7 +1877,7 @@
     </row>
     <row r="26" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="5">
         <v>18</v>
@@ -1794,10 +1886,10 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>7</v>
@@ -2064,14 +2156,340 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69FB0F7-484B-492C-A397-7FB7EAB5F35E}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="36">
+        <v>9</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="3">
+        <v>18</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="34">
+        <v>9</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="3">
+        <v>18</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="3">
+        <v>18</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified bash; other trial simulations
</commit_message>
<xml_diff>
--- a/Simulations/SimulationsLog.xlsx
+++ b/Simulations/SimulationsLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\OneDrive - Politecnico di Milano\Documenti\Università\2022-2023 - Quinto Anno\Computational Fluid Dynamics\Project\progetto_CFD\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF34605A-9E91-4914-90A3-FC30ABBDA0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB85AD88-C89F-43F5-A86B-556EB3DA2A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid Properties &amp; Calculations" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="90">
   <si>
     <t>Mesh</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t>SST-V2033m with std boundary conditions</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>FDS - MUSCL ON - SL 0.05</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>JST default</t>
   </si>
 </sst>
 </file>
@@ -380,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -698,11 +716,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -793,6 +872,30 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1075,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB05BFA5-83D5-460F-8809-94ABF6EE4EEF}">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2156,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69FB0F7-484B-492C-A397-7FB7EAB5F35E}">
-  <dimension ref="B1:H31"/>
+  <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,13 +2271,13 @@
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
@@ -2193,11 +2296,17 @@
       <c r="G2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="40" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="s">
         <v>74</v>
       </c>
@@ -2213,11 +2322,13 @@
       <c r="G3" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="47"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4" s="33" t="s">
         <v>78</v>
       </c>
@@ -2233,11 +2344,13 @@
       <c r="G4" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="48"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>79</v>
       </c>
@@ -2253,11 +2366,13 @@
       <c r="G5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>80</v>
       </c>
@@ -2273,11 +2388,13 @@
       <c r="G6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>82</v>
       </c>
@@ -2293,201 +2410,275 @@
       <c r="G7" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="48"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="3">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="3">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="43"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="48"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="43"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="48"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="43"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="48"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="43"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="48"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="43"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="48"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="43"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="43"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="48"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="43"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="48"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="43"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="48"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="43"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="48"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="43"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="48"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="43"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="48"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="43"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="48"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="43"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="48"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="43"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="48"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="43"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="48"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="43"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="48"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="43"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="48"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="43"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="48"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="43"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="48"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="43"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="48"/>
+    </row>
+    <row r="31" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made trial simulations with SST turbulence model
</commit_message>
<xml_diff>
--- a/Simulations/SimulationsLog.xlsx
+++ b/Simulations/SimulationsLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\OneDrive - Politecnico di Milano\Documenti\Università\2022-2023 - Quinto Anno\Computational Fluid Dynamics\Project\progetto_CFD\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB85AD88-C89F-43F5-A86B-556EB3DA2A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41ADDEB-0287-4002-898E-EB49BB80E981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24708" yWindow="2736" windowWidth="21600" windowHeight="11292" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid Properties &amp; Calculations" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="86">
   <si>
     <t>Mesh</t>
   </si>
@@ -152,9 +152,6 @@
     <t>selected_TURBULENCEINTENSITY</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>SA BOUNDARY CONDITIONS [SI]</t>
   </si>
   <si>
@@ -263,52 +260,43 @@
     <t>meshG3</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>Folder: SC</t>
   </si>
   <si>
     <t>Folder: P</t>
   </si>
   <si>
-    <t>SST-V2033m-VORTICITY-SUSTAINING with std boundary conditions</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>SST-V2033m with std boundary conditions</t>
-  </si>
-  <si>
     <t>Cl</t>
   </si>
   <si>
     <t>Cd</t>
   </si>
   <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>FDS - MUSCL ON - SL 0.05</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>JST default</t>
+    <t>SSTINV_OPT1</t>
+  </si>
+  <si>
+    <t>SSTINV_OPT2</t>
+  </si>
+  <si>
+    <t>SSTINV_OPT3</t>
+  </si>
+  <si>
+    <t>SSTINV_OPT4</t>
+  </si>
+  <si>
+    <t>SST-v2003m-VORTICITY-SUSTAINING with std bcs</t>
+  </si>
+  <si>
+    <t>SST-v2003m with std bcs</t>
+  </si>
+  <si>
+    <t>SST-v2003m-VORTICITY with std bcs</t>
+  </si>
+  <si>
+    <t>SST-v2003m-SUSTAINING with std bcs</t>
+  </si>
+  <si>
+    <t>FDS - MUSCL ON - TVD 0.05</t>
   </si>
 </sst>
 </file>
@@ -781,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -896,6 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1178,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB05BFA5-83D5-460F-8809-94ABF6EE4EEF}">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,10 +1190,10 @@
         <v>1.2</v>
       </c>
       <c r="H2" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="J2" s="10">
         <v>40176</v>
@@ -1218,7 +1207,7 @@
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1231,7 +1220,7 @@
         <v>1.9199999999999999E-5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -1243,25 +1232,25 @@
         <v>1.008</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="4">
         <v>9</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="4">
         <v>18</v>
@@ -1299,7 +1288,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -1380,25 +1369,25 @@
       <c r="C21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="21" t="s">
-        <v>37</v>
+      <c r="D21" s="21">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>37</v>
+      <c r="D22" s="23">
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="28">
         <v>0.21043799999999999</v>
@@ -1406,10 +1395,10 @@
     </row>
     <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="29">
         <v>1.2942340000000001</v>
@@ -1417,10 +1406,10 @@
     </row>
     <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="D26" s="27">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1497,7 +1486,7 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>13</v>
@@ -1600,7 +1589,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="36">
         <v>9</v>
@@ -1609,7 +1598,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="36" t="s">
         <v>14</v>
@@ -1620,7 +1609,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3">
         <v>9</v>
@@ -1629,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
@@ -1640,7 +1629,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3">
         <v>9</v>
@@ -1649,7 +1638,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1660,7 +1649,7 @@
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="5">
         <v>9</v>
@@ -1669,7 +1658,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>14</v>
@@ -1680,7 +1669,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="36">
         <v>9</v>
@@ -1689,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="36" t="s">
         <v>14</v>
@@ -1700,7 +1689,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3">
         <v>9</v>
@@ -1709,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>14</v>
@@ -1720,7 +1709,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3">
         <v>9</v>
@@ -1729,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>14</v>
@@ -1740,7 +1729,7 @@
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="37">
         <v>9</v>
@@ -1749,7 +1738,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="37" t="s">
         <v>14</v>
@@ -1760,7 +1749,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="36">
         <v>18</v>
@@ -1780,7 +1769,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="3">
         <v>18</v>
@@ -1800,7 +1789,7 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3">
         <v>18</v>
@@ -1820,7 +1809,7 @@
     </row>
     <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="37">
         <v>18</v>
@@ -1840,7 +1829,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="36">
         <v>18</v>
@@ -1849,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>14</v>
@@ -1860,7 +1849,7 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3">
         <v>18</v>
@@ -1869,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>14</v>
@@ -1880,7 +1869,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3">
         <v>18</v>
@@ -1889,7 +1878,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>14</v>
@@ -1900,7 +1889,7 @@
     </row>
     <row r="22" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="37">
         <v>18</v>
@@ -1909,7 +1898,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="37" t="s">
         <v>14</v>
@@ -1920,7 +1909,7 @@
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="36">
         <v>18</v>
@@ -1929,7 +1918,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="36" t="s">
         <v>14</v>
@@ -1940,7 +1929,7 @@
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3">
         <v>18</v>
@@ -1949,7 +1938,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>14</v>
@@ -1960,7 +1949,7 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3">
         <v>18</v>
@@ -1969,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>14</v>
@@ -1980,7 +1969,7 @@
     </row>
     <row r="26" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5">
         <v>18</v>
@@ -1989,7 +1978,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>14</v>
@@ -2261,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69FB0F7-484B-492C-A397-7FB7EAB5F35E}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,7 +2260,7 @@
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2279,7 +2268,7 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>13</v>
@@ -2300,33 +2289,37 @@
         <v>15</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D3" s="36">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E3" s="36" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="47"/>
+      <c r="I3" s="9">
+        <v>0.61174300000000004</v>
+      </c>
+      <c r="J3" s="47">
+        <v>0.16929</v>
+      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4" s="33" t="s">
@@ -2339,41 +2332,49 @@
         <v>3</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="48"/>
+      <c r="I4" s="1">
+        <v>1.147983</v>
+      </c>
+      <c r="J4" s="48">
+        <v>0.151475</v>
+      </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="33" t="s">
         <v>79</v>
       </c>
       <c r="D5" s="34">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="48"/>
+      <c r="I5" s="1">
+        <v>1.1599699999999999</v>
+      </c>
+      <c r="J5" s="50">
+        <v>0.15068699999999999</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="33" t="s">
         <v>80</v>
       </c>
       <c r="D6" s="3">
@@ -2383,33 +2384,27 @@
         <v>3</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="48"/>
+      <c r="I6" s="1">
+        <v>0.61143700000000001</v>
+      </c>
+      <c r="J6" s="48">
+        <v>0.16935</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="3">
-        <v>18</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>83</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="43" t="s">
         <v>7</v>
       </c>
@@ -2417,21 +2412,11 @@
       <c r="J7" s="48"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="3">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>77</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="43" t="s">
         <v>7</v>
       </c>
@@ -2439,21 +2424,11 @@
       <c r="J8" s="48"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="3">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>77</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="43" t="s">
         <v>7</v>
       </c>
@@ -2682,5 +2657,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New mesh convergence bash script; new trial simulations for SST turbulence model
</commit_message>
<xml_diff>
--- a/Simulations/SimulationsLog.xlsx
+++ b/Simulations/SimulationsLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\OneDrive - Politecnico di Milano\Documenti\Università\2022-2023 - Quinto Anno\Computational Fluid Dynamics\Project\progetto_CFD\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41ADDEB-0287-4002-898E-EB49BB80E981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D22D923-F4A8-466A-A5C5-BCC9DD0C59FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24708" yWindow="2736" windowWidth="21600" windowHeight="11292" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="2565" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid Properties &amp; Calculations" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Mesh</t>
   </si>
@@ -272,18 +272,6 @@
     <t>Cd</t>
   </si>
   <si>
-    <t>SSTINV_OPT1</t>
-  </si>
-  <si>
-    <t>SSTINV_OPT2</t>
-  </si>
-  <si>
-    <t>SSTINV_OPT3</t>
-  </si>
-  <si>
-    <t>SSTINV_OPT4</t>
-  </si>
-  <si>
     <t>SST-v2003m-VORTICITY-SUSTAINING with std bcs</t>
   </si>
   <si>
@@ -297,6 +285,27 @@
   </si>
   <si>
     <t>FDS - MUSCL ON - TVD 0.05</t>
+  </si>
+  <si>
+    <t>Goal and notes</t>
+  </si>
+  <si>
+    <t>Figure out the correct screen and history output configuration</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>SST_OPT1</t>
+  </si>
+  <si>
+    <t>SST_OPT2</t>
+  </si>
+  <si>
+    <t>SST_OPT3</t>
+  </si>
+  <si>
+    <t>SST_OPT4</t>
   </si>
 </sst>
 </file>
@@ -769,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -863,12 +872,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,10 +884,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1167,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB05BFA5-83D5-460F-8809-94ABF6EE4EEF}">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1467,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H56"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2248,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69FB0F7-484B-492C-A397-7FB7EAB5F35E}">
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,10 +2304,11 @@
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>74</v>
       </c>
@@ -2288,94 +2330,85 @@
       <c r="H2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="44" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="K2" s="47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="50">
+        <v>18</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="36">
+      <c r="H3" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="52"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="54">
         <v>18</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E4" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="36" t="s">
+      <c r="F4" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.61174300000000004</v>
-      </c>
-      <c r="J3" s="47">
-        <v>0.16929</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="33" t="s">
+      <c r="G4" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3">
+      <c r="H4" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="55">
         <v>18</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E5" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1.147983</v>
-      </c>
-      <c r="J4" s="48">
-        <v>0.151475</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="33" t="s">
+      <c r="F5" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="34">
-        <v>18</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1.1599699999999999</v>
-      </c>
-      <c r="J5" s="50">
-        <v>0.15068699999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="57"/>
+      <c r="J5" s="60"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="33" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D6" s="3">
         <v>18</v>
@@ -2384,126 +2417,139 @@
         <v>3</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="49"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.61143700000000001</v>
-      </c>
-      <c r="J6" s="48">
-        <v>0.16935</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="48"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>18</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="48"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="49"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="34"/>
-      <c r="H9" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="48"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="49"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="48"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="41"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="48"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="41"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="48"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="41"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="48"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="41"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="48"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="41"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="48"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="41"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="48"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -2511,9 +2557,9 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
@@ -2521,9 +2567,9 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
@@ -2531,9 +2577,9 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
@@ -2541,9 +2587,9 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="48"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -2551,9 +2597,9 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="48"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
@@ -2561,9 +2607,9 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="48"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
@@ -2571,9 +2617,9 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="48"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
@@ -2581,9 +2627,9 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="48"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -2591,9 +2637,9 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="48"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
@@ -2601,9 +2647,9 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="48"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
@@ -2611,9 +2657,9 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="48"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
@@ -2621,9 +2667,9 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="48"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
@@ -2631,9 +2677,9 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="48"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
@@ -2641,9 +2687,9 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="43"/>
+      <c r="H30" s="41"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="48"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
@@ -2651,9 +2697,9 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="44"/>
+      <c r="H31" s="42"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="49"/>
+      <c r="J31" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>